<commit_message>
Data source corrected and updated
</commit_message>
<xml_diff>
--- a/data/group-a-1.xlsx
+++ b/data/group-a-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nirmal/Documents/ML_DS/ml_dsc_cell/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nirmal/Documents/data_science/microDSC_error_prediction_ANN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC0D77-8D7F-084C-8680-1B3B42B17F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB895F77-BCF3-2545-9F67-2A5202D38134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18840" windowHeight="12460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -84,7 +77,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -372,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,8 +375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -416,11 +409,11 @@
       <c r="I1">
         <v>1.2757350000000001</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>0.3</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -452,10 +445,10 @@
         <v>1.2789550000000001</v>
       </c>
       <c r="J2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
@@ -487,10 +480,10 @@
         <v>1.2797620000000001</v>
       </c>
       <c r="J3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
@@ -522,10 +515,10 @@
         <v>1.2816369999999999</v>
       </c>
       <c r="J4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -557,10 +550,10 @@
         <v>1.2829619999999999</v>
       </c>
       <c r="J5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -592,10 +585,10 @@
         <v>1.284211</v>
       </c>
       <c r="J6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -627,10 +620,10 @@
         <v>1.285156</v>
       </c>
       <c r="J7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -662,10 +655,10 @@
         <v>1.2866850000000001</v>
       </c>
       <c r="J8">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -697,10 +690,10 @@
         <v>1.2879130000000001</v>
       </c>
       <c r="J9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -732,10 +725,10 @@
         <v>1.2893619999999999</v>
       </c>
       <c r="J10">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -767,10 +760,10 @@
         <v>1.2908090000000001</v>
       </c>
       <c r="J11">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -802,10 +795,10 @@
         <v>1.2914410000000001</v>
       </c>
       <c r="J12">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -837,10 +830,10 @@
         <v>1.2931299999999999</v>
       </c>
       <c r="J13">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -872,10 +865,10 @@
         <v>1.294244</v>
       </c>
       <c r="J14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -907,10 +900,10 @@
         <v>1.2957069999999999</v>
       </c>
       <c r="J15">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -942,10 +935,10 @@
         <v>1.2970839999999999</v>
       </c>
       <c r="J16">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -977,10 +970,10 @@
         <v>1.2985789999999999</v>
       </c>
       <c r="J17">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1012,10 +1005,10 @@
         <v>1.2996049999999999</v>
       </c>
       <c r="J18">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1047,10 +1040,10 @@
         <v>1.301077</v>
       </c>
       <c r="J19">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1082,10 +1075,10 @@
         <v>1.3029280000000001</v>
       </c>
       <c r="J20">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
@@ -1117,10 +1110,10 @@
         <v>1.3034429999999999</v>
       </c>
       <c r="J21">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
@@ -1152,10 +1145,10 @@
         <v>1.304559</v>
       </c>
       <c r="J22">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
@@ -1187,10 +1180,10 @@
         <v>1.305895</v>
       </c>
       <c r="J23">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -1222,10 +1215,10 @@
         <v>1.3077700000000001</v>
       </c>
       <c r="J24">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
@@ -1257,10 +1250,10 @@
         <v>1.308565</v>
       </c>
       <c r="J25">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
@@ -1292,10 +1285,10 @@
         <v>1.3102720000000001</v>
       </c>
       <c r="J26">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
@@ -1327,10 +1320,10 @@
         <v>1.311458</v>
       </c>
       <c r="J27">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
@@ -1362,10 +1355,10 @@
         <v>1.3127740000000001</v>
       </c>
       <c r="J28">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
@@ -1397,10 +1390,10 @@
         <v>1.3135559999999999</v>
       </c>
       <c r="J29">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
@@ -1432,10 +1425,10 @@
         <v>1.3142389999999999</v>
       </c>
       <c r="J30">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
@@ -1467,10 +1460,10 @@
         <v>1.315445</v>
       </c>
       <c r="J31">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
@@ -1502,10 +1495,10 @@
         <v>1.3171029999999999</v>
       </c>
       <c r="J32">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
@@ -1537,10 +1530,10 @@
         <v>1.3181909999999999</v>
       </c>
       <c r="J33">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
@@ -1572,10 +1565,10 @@
         <v>1.3198570000000001</v>
       </c>
       <c r="J34">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
@@ -1607,10 +1600,10 @@
         <v>1.321286</v>
       </c>
       <c r="J35">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
@@ -1642,10 +1635,10 @@
         <v>1.3225560000000001</v>
       </c>
       <c r="J36">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
@@ -1677,10 +1670,10 @@
         <v>1.3240670000000001</v>
       </c>
       <c r="J37">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
@@ -1712,10 +1705,10 @@
         <v>1.325691</v>
       </c>
       <c r="J38">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
@@ -1747,10 +1740,10 @@
         <v>1.3260749999999999</v>
       </c>
       <c r="J39">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
@@ -1782,10 +1775,10 @@
         <v>1.3279570000000001</v>
       </c>
       <c r="J40">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K40">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
@@ -1817,10 +1810,10 @@
         <v>1.3282080000000001</v>
       </c>
       <c r="J41">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
@@ -1852,10 +1845,10 @@
         <v>1.3293219999999999</v>
       </c>
       <c r="J42">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K42">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
@@ -1887,10 +1880,10 @@
         <v>1.3305389999999999</v>
       </c>
       <c r="J43">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K43">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -1922,10 +1915,10 @@
         <v>1.3322240000000001</v>
       </c>
       <c r="J44">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K44">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
@@ -1957,10 +1950,10 @@
         <v>1.3323020000000001</v>
       </c>
       <c r="J45">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K45">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.15">
@@ -1992,10 +1985,10 @@
         <v>1.3340080000000001</v>
       </c>
       <c r="J46">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.15">
@@ -2027,10 +2020,10 @@
         <v>1.334746</v>
       </c>
       <c r="J47">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K47">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
@@ -2062,10 +2055,10 @@
         <v>1.335745</v>
       </c>
       <c r="J48">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
@@ -2097,10 +2090,10 @@
         <v>1.336462</v>
       </c>
       <c r="J49">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
@@ -2132,10 +2125,10 @@
         <v>1.336916</v>
       </c>
       <c r="J50">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.15">
@@ -2167,10 +2160,10 @@
         <v>1.3381890000000001</v>
       </c>
       <c r="J51">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>